<commit_message>
Auto-committed on 2022/01/19 週三
Former-commit-id: d7df9c717f8b567b4f03227e194205307dc407d2
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L1-顧客管理作業/CustMain.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L1-顧客管理作業/CustMain.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L1-顧客管理作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7060490B-88B0-4850-A4D7-E4F30CC9BEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132"/>
+    <workbookView xWindow="6288" yWindow="48" windowWidth="16476" windowHeight="11412" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
     <sheet name="DBS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -812,10 +813,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>法人:營業地國籍</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>DataStatus</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -909,11 +906,15 @@
     <t>IncomeDataDate</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>自然人:居住地國籍/法人:營業地國籍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1189,7 +1190,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2" xfId="1"/>
+    <cellStyle name="一般 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1280,6 +1281,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1315,6 +1333,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1490,11 +1525,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -1631,7 +1666,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>184</v>
@@ -1797,7 +1832,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>7</v>
@@ -1822,7 +1857,7 @@
         <v>189</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>10</v>
@@ -1844,7 +1879,7 @@
         <v>190</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>10</v>
@@ -2391,20 +2426,20 @@
         <v>38</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E46" s="25">
         <v>1</v>
       </c>
       <c r="F46" s="25"/>
       <c r="G46" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
@@ -2416,7 +2451,7 @@
         <v>95</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D47" s="18" t="s">
         <v>10</v>
@@ -2426,7 +2461,7 @@
       </c>
       <c r="F47" s="18"/>
       <c r="G47" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="1:7" s="1" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
@@ -2641,7 +2676,7 @@
         <v>50</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C58" s="24" t="s">
         <v>161</v>
@@ -2786,7 +2821,7 @@
         <v>148</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D65" s="24" t="s">
         <v>158</v>
@@ -2796,7 +2831,7 @@
       </c>
       <c r="F65" s="24"/>
       <c r="G65" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2847,7 +2882,7 @@
         <v>60</v>
       </c>
       <c r="B68" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C68" s="28" t="s">
         <v>160</v>
@@ -2916,7 +2951,7 @@
         <v>176</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D71" s="25" t="s">
         <v>10</v>
@@ -2935,7 +2970,7 @@
         <v>64</v>
       </c>
       <c r="B72" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C72" s="28" t="s">
         <v>183</v>
@@ -2948,7 +2983,7 @@
       </c>
       <c r="F72" s="29"/>
       <c r="G72" s="28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="81" x14ac:dyDescent="0.3">
@@ -2970,7 +3005,7 @@
       </c>
       <c r="F73" s="29"/>
       <c r="G73" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -3051,7 +3086,7 @@
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D84" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.3">
@@ -3077,7 +3112,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
@@ -3136,7 +3171,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>129</v>
@@ -3185,10 +3220,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>147</v>

</xml_diff>